<commit_message>
Added manual investigations of individual tool settings
</commit_message>
<xml_diff>
--- a/GOLD_indv_nicad_df_090301.xlsx
+++ b/GOLD_indv_nicad_df_090301.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="6380" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="indv_nicad_df_090301" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="595">
   <si>
     <t>stackoverflow_formatted/10299606_0.java</t>
   </si>
@@ -1770,6 +1770,48 @@
   </si>
   <si>
     <t>jasperreports-3/jasperreports-3.7.4/src/net/sf/jasperreports/engine/design/JRJdtCompiler.java</t>
+  </si>
+  <si>
+    <t>similar equals() method</t>
+  </si>
+  <si>
+    <t>similar implementation of binary search (SO answer is removed)</t>
+  </si>
+  <si>
+    <t>false clone</t>
+  </si>
+  <si>
+    <t>similar finally clause after normalisation</t>
+  </si>
+  <si>
+    <t>similar code after normalisation</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>SO answer is copied from http://tech.groups.yahoo.com/group/Firebird-Java/message/10715 but the CachedRowSetImpl is in Compiere (it is actually from com.sun.rowset.CachedRowSetImpl).</t>
+  </si>
+  <si>
+    <t>similar implementation of compare() method</t>
+  </si>
+  <si>
+    <t>similar try-catch clause</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>both classes extend from HTMLEditorKit and have similar createDefaultDocument() method</t>
+  </si>
+  <si>
+    <t>similar Iterator code</t>
+  </si>
+  <si>
+    <t>similar implementation of indexOf() and getIndexOf() methods</t>
+  </si>
+  <si>
+    <t>similar getInstance() method after normalisation</t>
   </si>
 </sst>
 </file>
@@ -2086,11 +2128,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="O276" sqref="O276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.83203125" customWidth="1"/>
+    <col min="5" max="7" width="6" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="36.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3771,7 +3822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>372</v>
       </c>
@@ -3797,7 +3848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>434</v>
       </c>
@@ -3823,7 +3874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>458</v>
       </c>
@@ -3849,7 +3900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>528</v>
       </c>
@@ -3875,7 +3926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>535</v>
       </c>
@@ -3901,7 +3952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>557</v>
       </c>
@@ -3923,8 +3974,14 @@
       <c r="G70">
         <v>19</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" t="s">
+        <v>294</v>
+      </c>
+      <c r="J70" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -3946,8 +4003,14 @@
       <c r="G71">
         <v>16</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" t="s">
+        <v>294</v>
+      </c>
+      <c r="J71" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3969,8 +4032,14 @@
       <c r="G72">
         <v>16</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" t="s">
+        <v>294</v>
+      </c>
+      <c r="J72" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>262</v>
       </c>
@@ -3992,8 +4061,14 @@
       <c r="G73">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" t="s">
+        <v>294</v>
+      </c>
+      <c r="J73" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>352</v>
       </c>
@@ -4015,8 +4090,14 @@
       <c r="G74">
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>294</v>
+      </c>
+      <c r="J74" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>410</v>
       </c>
@@ -4038,8 +4119,14 @@
       <c r="G75">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>294</v>
+      </c>
+      <c r="J75" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>430</v>
       </c>
@@ -4061,8 +4148,14 @@
       <c r="G76">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>294</v>
+      </c>
+      <c r="J76" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>490</v>
       </c>
@@ -4084,8 +4177,14 @@
       <c r="G77">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" t="s">
+        <v>294</v>
+      </c>
+      <c r="J77" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>392</v>
       </c>
@@ -4107,8 +4206,14 @@
       <c r="G78">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" t="s">
+        <v>230</v>
+      </c>
+      <c r="J78" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>452</v>
       </c>
@@ -4130,8 +4235,14 @@
       <c r="G79">
         <v>15</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" t="s">
+        <v>230</v>
+      </c>
+      <c r="J79" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>125</v>
       </c>
@@ -4153,8 +4264,14 @@
       <c r="G80">
         <v>14</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I80" t="s">
+        <v>230</v>
+      </c>
+      <c r="J80" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>340</v>
       </c>
@@ -4176,8 +4293,14 @@
       <c r="G81">
         <v>14</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I81" t="s">
+        <v>230</v>
+      </c>
+      <c r="J81" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>63</v>
       </c>
@@ -4199,8 +4322,14 @@
       <c r="G82">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I82" t="s">
+        <v>294</v>
+      </c>
+      <c r="J82" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>69</v>
       </c>
@@ -4222,8 +4351,14 @@
       <c r="G83">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I83" t="s">
+        <v>230</v>
+      </c>
+      <c r="J83" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -4245,8 +4380,14 @@
       <c r="G84">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I84" t="s">
+        <v>586</v>
+      </c>
+      <c r="J84" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>318</v>
       </c>
@@ -4268,8 +4409,14 @@
       <c r="G85">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I85" t="s">
+        <v>230</v>
+      </c>
+      <c r="J85" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>390</v>
       </c>
@@ -4291,8 +4438,14 @@
       <c r="G86">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I86" t="s">
+        <v>294</v>
+      </c>
+      <c r="J86" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -4314,8 +4467,14 @@
       <c r="G87">
         <v>12</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I87" t="s">
+        <v>230</v>
+      </c>
+      <c r="J87" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -4337,8 +4496,14 @@
       <c r="G88">
         <v>12</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I88" t="s">
+        <v>230</v>
+      </c>
+      <c r="J88" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>39</v>
       </c>
@@ -4360,8 +4525,14 @@
       <c r="G89">
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I89" t="s">
+        <v>230</v>
+      </c>
+      <c r="J89" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>59</v>
       </c>
@@ -4383,8 +4554,14 @@
       <c r="G90">
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I90" t="s">
+        <v>294</v>
+      </c>
+      <c r="J90" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -4406,8 +4583,14 @@
       <c r="G91">
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I91" t="s">
+        <v>230</v>
+      </c>
+      <c r="J91" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>127</v>
       </c>
@@ -4429,8 +4612,14 @@
       <c r="G92">
         <v>12</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I92" t="s">
+        <v>230</v>
+      </c>
+      <c r="J92" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -4452,8 +4641,14 @@
       <c r="G93">
         <v>12</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I93" t="s">
+        <v>230</v>
+      </c>
+      <c r="J93" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>145</v>
       </c>
@@ -4475,8 +4670,14 @@
       <c r="G94">
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I94" t="s">
+        <v>230</v>
+      </c>
+      <c r="J94" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>161</v>
       </c>
@@ -4498,8 +4699,14 @@
       <c r="G95">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I95" t="s">
+        <v>230</v>
+      </c>
+      <c r="J95" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>183</v>
       </c>
@@ -4521,8 +4728,14 @@
       <c r="G96">
         <v>12</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I96" t="s">
+        <v>294</v>
+      </c>
+      <c r="J96" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>238</v>
       </c>
@@ -4544,8 +4757,14 @@
       <c r="G97">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I97" t="s">
+        <v>230</v>
+      </c>
+      <c r="J97" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>258</v>
       </c>
@@ -4567,8 +4786,14 @@
       <c r="G98">
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I98" t="s">
+        <v>230</v>
+      </c>
+      <c r="J98" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>264</v>
       </c>
@@ -4590,8 +4815,14 @@
       <c r="G99">
         <v>12</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I99" t="s">
+        <v>230</v>
+      </c>
+      <c r="J99" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>272</v>
       </c>
@@ -4613,8 +4844,14 @@
       <c r="G100">
         <v>12</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I100" t="s">
+        <v>294</v>
+      </c>
+      <c r="J100" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>328</v>
       </c>
@@ -4636,8 +4873,14 @@
       <c r="G101">
         <v>12</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I101" t="s">
+        <v>230</v>
+      </c>
+      <c r="J101" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>420</v>
       </c>
@@ -4659,8 +4902,14 @@
       <c r="G102">
         <v>12</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I102" t="s">
+        <v>230</v>
+      </c>
+      <c r="J102" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>464</v>
       </c>
@@ -4682,8 +4931,14 @@
       <c r="G103">
         <v>12</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I103" t="s">
+        <v>230</v>
+      </c>
+      <c r="J103" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>466</v>
       </c>
@@ -4705,8 +4960,14 @@
       <c r="G104">
         <v>12</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I104" t="s">
+        <v>230</v>
+      </c>
+      <c r="J104" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>476</v>
       </c>
@@ -4728,8 +4989,14 @@
       <c r="G105">
         <v>12</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I105" t="s">
+        <v>230</v>
+      </c>
+      <c r="J105" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>482</v>
       </c>
@@ -4751,8 +5018,14 @@
       <c r="G106">
         <v>12</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I106" t="s">
+        <v>230</v>
+      </c>
+      <c r="J106" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>484</v>
       </c>
@@ -4774,8 +5047,14 @@
       <c r="G107">
         <v>12</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I107" t="s">
+        <v>230</v>
+      </c>
+      <c r="J107" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>492</v>
       </c>
@@ -4797,8 +5076,14 @@
       <c r="G108">
         <v>12</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I108" t="s">
+        <v>230</v>
+      </c>
+      <c r="J108" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>510</v>
       </c>
@@ -4820,8 +5105,14 @@
       <c r="G109">
         <v>12</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I109" t="s">
+        <v>230</v>
+      </c>
+      <c r="J109" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>559</v>
       </c>
@@ -4843,8 +5134,14 @@
       <c r="G110">
         <v>12</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I110" t="s">
+        <v>230</v>
+      </c>
+      <c r="J110" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>563</v>
       </c>
@@ -4866,8 +5163,14 @@
       <c r="G111">
         <v>12</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I111" t="s">
+        <v>230</v>
+      </c>
+      <c r="J111" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>573</v>
       </c>
@@ -4889,8 +5192,14 @@
       <c r="G112">
         <v>12</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I112" t="s">
+        <v>230</v>
+      </c>
+      <c r="J112" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>17</v>
       </c>
@@ -4912,8 +5221,14 @@
       <c r="G113">
         <v>11</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I113" t="s">
+        <v>230</v>
+      </c>
+      <c r="J113" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>19</v>
       </c>
@@ -4935,8 +5250,14 @@
       <c r="G114">
         <v>11</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I114" t="s">
+        <v>230</v>
+      </c>
+      <c r="J114" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>37</v>
       </c>
@@ -4958,8 +5279,14 @@
       <c r="G115">
         <v>11</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I115" t="s">
+        <v>230</v>
+      </c>
+      <c r="J115" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>71</v>
       </c>
@@ -4981,8 +5308,14 @@
       <c r="G116">
         <v>11</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I116" t="s">
+        <v>230</v>
+      </c>
+      <c r="J116" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>75</v>
       </c>
@@ -5004,8 +5337,14 @@
       <c r="G117">
         <v>11</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I117" t="s">
+        <v>230</v>
+      </c>
+      <c r="J117" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>87</v>
       </c>
@@ -5027,8 +5366,14 @@
       <c r="G118">
         <v>11</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I118" t="s">
+        <v>230</v>
+      </c>
+      <c r="J118" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>97</v>
       </c>
@@ -5050,8 +5395,14 @@
       <c r="G119">
         <v>11</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I119" t="s">
+        <v>230</v>
+      </c>
+      <c r="J119" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>99</v>
       </c>
@@ -5073,8 +5424,14 @@
       <c r="G120">
         <v>11</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I120" t="s">
+        <v>230</v>
+      </c>
+      <c r="J120" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>149</v>
       </c>
@@ -5096,8 +5453,14 @@
       <c r="G121">
         <v>11</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I121" t="s">
+        <v>230</v>
+      </c>
+      <c r="J121" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>151</v>
       </c>
@@ -5119,8 +5482,14 @@
       <c r="G122">
         <v>11</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I122" t="s">
+        <v>230</v>
+      </c>
+      <c r="J122" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>153</v>
       </c>
@@ -5142,8 +5511,14 @@
       <c r="G123">
         <v>11</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I123" t="s">
+        <v>294</v>
+      </c>
+      <c r="J123" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>157</v>
       </c>
@@ -5165,8 +5540,14 @@
       <c r="G124">
         <v>11</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I124" t="s">
+        <v>294</v>
+      </c>
+      <c r="J124" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>165</v>
       </c>
@@ -5188,8 +5569,14 @@
       <c r="G125">
         <v>11</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I125" t="s">
+        <v>230</v>
+      </c>
+      <c r="J125" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>173</v>
       </c>
@@ -5211,8 +5598,14 @@
       <c r="G126">
         <v>11</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I126" t="s">
+        <v>230</v>
+      </c>
+      <c r="J126" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>181</v>
       </c>
@@ -5234,8 +5627,14 @@
       <c r="G127">
         <v>11</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I127" t="s">
+        <v>230</v>
+      </c>
+      <c r="J127" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>211</v>
       </c>
@@ -5257,8 +5656,14 @@
       <c r="G128">
         <v>11</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I128" t="s">
+        <v>230</v>
+      </c>
+      <c r="J128" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>219</v>
       </c>
@@ -5280,8 +5685,14 @@
       <c r="G129">
         <v>11</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I129" t="s">
+        <v>230</v>
+      </c>
+      <c r="J129" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>248</v>
       </c>
@@ -5303,8 +5714,14 @@
       <c r="G130">
         <v>11</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I130" t="s">
+        <v>230</v>
+      </c>
+      <c r="J130" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>260</v>
       </c>
@@ -5326,8 +5743,14 @@
       <c r="G131">
         <v>11</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I131" t="s">
+        <v>230</v>
+      </c>
+      <c r="J131" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>266</v>
       </c>
@@ -5349,8 +5772,14 @@
       <c r="G132">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I132" t="s">
+        <v>230</v>
+      </c>
+      <c r="J132" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>268</v>
       </c>
@@ -5372,8 +5801,14 @@
       <c r="G133">
         <v>11</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I133" t="s">
+        <v>230</v>
+      </c>
+      <c r="J133" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>290</v>
       </c>
@@ -5395,8 +5830,14 @@
       <c r="G134">
         <v>11</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I134" t="s">
+        <v>294</v>
+      </c>
+      <c r="J134" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>296</v>
       </c>
@@ -5418,8 +5859,14 @@
       <c r="G135">
         <v>11</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I135" t="s">
+        <v>230</v>
+      </c>
+      <c r="J135" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>314</v>
       </c>
@@ -5441,8 +5888,14 @@
       <c r="G136">
         <v>11</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I136" t="s">
+        <v>230</v>
+      </c>
+      <c r="J136" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>342</v>
       </c>
@@ -5464,8 +5917,14 @@
       <c r="G137">
         <v>11</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I137" t="s">
+        <v>230</v>
+      </c>
+      <c r="J137" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>346</v>
       </c>
@@ -5487,8 +5946,14 @@
       <c r="G138">
         <v>11</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I138" t="s">
+        <v>230</v>
+      </c>
+      <c r="J138" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>362</v>
       </c>
@@ -5510,8 +5975,14 @@
       <c r="G139">
         <v>11</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I139" t="s">
+        <v>294</v>
+      </c>
+      <c r="J139" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>398</v>
       </c>
@@ -5533,8 +6004,14 @@
       <c r="G140">
         <v>11</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I140" t="s">
+        <v>230</v>
+      </c>
+      <c r="J140" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>416</v>
       </c>
@@ -5556,8 +6033,14 @@
       <c r="G141">
         <v>11</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I141" t="s">
+        <v>230</v>
+      </c>
+      <c r="J141" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>444</v>
       </c>
@@ -5579,8 +6062,14 @@
       <c r="G142">
         <v>11</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I142" t="s">
+        <v>230</v>
+      </c>
+      <c r="J142" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>474</v>
       </c>
@@ -5602,8 +6091,14 @@
       <c r="G143">
         <v>11</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I143" t="s">
+        <v>230</v>
+      </c>
+      <c r="J143" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>486</v>
       </c>
@@ -5625,8 +6120,14 @@
       <c r="G144">
         <v>11</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I144" t="s">
+        <v>230</v>
+      </c>
+      <c r="J144" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>496</v>
       </c>
@@ -5648,8 +6149,14 @@
       <c r="G145">
         <v>11</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I145" t="s">
+        <v>230</v>
+      </c>
+      <c r="J145" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>512</v>
       </c>
@@ -5671,8 +6178,14 @@
       <c r="G146">
         <v>11</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I146" t="s">
+        <v>230</v>
+      </c>
+      <c r="J146" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>530</v>
       </c>
@@ -5694,8 +6207,14 @@
       <c r="G147">
         <v>11</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I147" t="s">
+        <v>230</v>
+      </c>
+      <c r="J147" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>543</v>
       </c>
@@ -5717,8 +6236,14 @@
       <c r="G148">
         <v>11</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I148" t="s">
+        <v>230</v>
+      </c>
+      <c r="J148" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>545</v>
       </c>
@@ -5740,8 +6265,14 @@
       <c r="G149">
         <v>11</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I149" t="s">
+        <v>230</v>
+      </c>
+      <c r="J149" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>547</v>
       </c>
@@ -5763,8 +6294,14 @@
       <c r="G150">
         <v>11</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I150" t="s">
+        <v>294</v>
+      </c>
+      <c r="J150" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>549</v>
       </c>
@@ -5786,8 +6323,14 @@
       <c r="G151">
         <v>11</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I151" t="s">
+        <v>230</v>
+      </c>
+      <c r="J151" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>553</v>
       </c>
@@ -5809,8 +6352,14 @@
       <c r="G152">
         <v>11</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I152" t="s">
+        <v>230</v>
+      </c>
+      <c r="J152" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>565</v>
       </c>
@@ -5832,8 +6381,14 @@
       <c r="G153">
         <v>11</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I153" t="s">
+        <v>230</v>
+      </c>
+      <c r="J153" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>575</v>
       </c>
@@ -5855,8 +6410,14 @@
       <c r="G154">
         <v>11</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I154" t="s">
+        <v>230</v>
+      </c>
+      <c r="J154" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>579</v>
       </c>
@@ -5878,8 +6439,14 @@
       <c r="G155">
         <v>11</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I155" t="s">
+        <v>230</v>
+      </c>
+      <c r="J155" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>5</v>
       </c>
@@ -5901,8 +6468,14 @@
       <c r="G156">
         <v>10</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I156" t="s">
+        <v>590</v>
+      </c>
+      <c r="J156" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>13</v>
       </c>
@@ -5924,8 +6497,14 @@
       <c r="G157">
         <v>10</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I157" t="s">
+        <v>230</v>
+      </c>
+      <c r="J157" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>23</v>
       </c>
@@ -5947,8 +6526,14 @@
       <c r="G158">
         <v>10</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I158" t="s">
+        <v>230</v>
+      </c>
+      <c r="J158" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>29</v>
       </c>
@@ -5970,8 +6555,14 @@
       <c r="G159">
         <v>10</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I159" t="s">
+        <v>230</v>
+      </c>
+      <c r="J159" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>33</v>
       </c>
@@ -5993,8 +6584,14 @@
       <c r="G160">
         <v>10</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I160" t="s">
+        <v>230</v>
+      </c>
+      <c r="J160" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>35</v>
       </c>
@@ -6016,8 +6613,14 @@
       <c r="G161">
         <v>10</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I161" t="s">
+        <v>230</v>
+      </c>
+      <c r="J161" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>41</v>
       </c>
@@ -6039,8 +6642,14 @@
       <c r="G162">
         <v>10</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I162" t="s">
+        <v>230</v>
+      </c>
+      <c r="J162" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>43</v>
       </c>
@@ -6062,8 +6671,14 @@
       <c r="G163">
         <v>10</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I163" t="s">
+        <v>230</v>
+      </c>
+      <c r="J163" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>47</v>
       </c>
@@ -6085,8 +6700,14 @@
       <c r="G164">
         <v>10</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I164" t="s">
+        <v>230</v>
+      </c>
+      <c r="J164" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>49</v>
       </c>
@@ -6108,8 +6729,14 @@
       <c r="G165">
         <v>10</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I165" t="s">
+        <v>230</v>
+      </c>
+      <c r="J165" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -6131,8 +6758,14 @@
       <c r="G166">
         <v>10</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I166" t="s">
+        <v>230</v>
+      </c>
+      <c r="J166" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>55</v>
       </c>
@@ -6154,8 +6787,14 @@
       <c r="G167">
         <v>10</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I167" t="s">
+        <v>294</v>
+      </c>
+      <c r="J167" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>57</v>
       </c>
@@ -6177,8 +6816,14 @@
       <c r="G168">
         <v>10</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I168" t="s">
+        <v>230</v>
+      </c>
+      <c r="J168" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>61</v>
       </c>
@@ -6200,8 +6845,14 @@
       <c r="G169">
         <v>10</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I169" t="s">
+        <v>294</v>
+      </c>
+      <c r="J169" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>67</v>
       </c>
@@ -6223,8 +6874,14 @@
       <c r="G170">
         <v>10</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I170" t="s">
+        <v>230</v>
+      </c>
+      <c r="J170" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>77</v>
       </c>
@@ -6246,8 +6903,14 @@
       <c r="G171">
         <v>10</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I171" t="s">
+        <v>294</v>
+      </c>
+      <c r="J171" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>79</v>
       </c>
@@ -6269,8 +6932,14 @@
       <c r="G172">
         <v>10</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I172" t="s">
+        <v>230</v>
+      </c>
+      <c r="J172" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>81</v>
       </c>
@@ -6292,8 +6961,14 @@
       <c r="G173">
         <v>10</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I173" t="s">
+        <v>230</v>
+      </c>
+      <c r="J173" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>89</v>
       </c>
@@ -6315,8 +6990,14 @@
       <c r="G174">
         <v>10</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I174" t="s">
+        <v>230</v>
+      </c>
+      <c r="J174" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>93</v>
       </c>
@@ -6338,8 +7019,14 @@
       <c r="G175">
         <v>10</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I175" t="s">
+        <v>230</v>
+      </c>
+      <c r="J175" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>95</v>
       </c>
@@ -6361,8 +7048,14 @@
       <c r="G176">
         <v>10</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I176" t="s">
+        <v>230</v>
+      </c>
+      <c r="J176" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>101</v>
       </c>
@@ -6384,8 +7077,14 @@
       <c r="G177">
         <v>10</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I177" t="s">
+        <v>230</v>
+      </c>
+      <c r="J177" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>103</v>
       </c>
@@ -6407,8 +7106,14 @@
       <c r="G178">
         <v>10</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I178" t="s">
+        <v>230</v>
+      </c>
+      <c r="J178" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>105</v>
       </c>
@@ -6430,8 +7135,14 @@
       <c r="G179">
         <v>10</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I179" t="s">
+        <v>230</v>
+      </c>
+      <c r="J179" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>109</v>
       </c>
@@ -6453,8 +7164,14 @@
       <c r="G180">
         <v>10</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I180" t="s">
+        <v>230</v>
+      </c>
+      <c r="J180" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>111</v>
       </c>
@@ -6476,8 +7193,14 @@
       <c r="G181">
         <v>10</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I181" t="s">
+        <v>294</v>
+      </c>
+      <c r="J181" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>113</v>
       </c>
@@ -6499,8 +7222,14 @@
       <c r="G182">
         <v>10</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I182" t="s">
+        <v>230</v>
+      </c>
+      <c r="J182" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>115</v>
       </c>
@@ -6522,8 +7251,14 @@
       <c r="G183">
         <v>10</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I183" t="s">
+        <v>230</v>
+      </c>
+      <c r="J183" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>117</v>
       </c>
@@ -6545,8 +7280,14 @@
       <c r="G184">
         <v>10</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I184" t="s">
+        <v>294</v>
+      </c>
+      <c r="J184" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>119</v>
       </c>
@@ -6568,8 +7309,14 @@
       <c r="G185">
         <v>10</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I185" t="s">
+        <v>230</v>
+      </c>
+      <c r="J185" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>121</v>
       </c>
@@ -6591,8 +7338,14 @@
       <c r="G186">
         <v>10</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I186" t="s">
+        <v>230</v>
+      </c>
+      <c r="J186" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>123</v>
       </c>
@@ -6614,8 +7367,14 @@
       <c r="G187">
         <v>10</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I187" t="s">
+        <v>230</v>
+      </c>
+      <c r="J187" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>129</v>
       </c>
@@ -6637,8 +7396,14 @@
       <c r="G188">
         <v>10</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I188" t="s">
+        <v>230</v>
+      </c>
+      <c r="J188" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>131</v>
       </c>
@@ -6660,8 +7425,14 @@
       <c r="G189">
         <v>10</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I189" t="s">
+        <v>230</v>
+      </c>
+      <c r="J189" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>137</v>
       </c>
@@ -6683,8 +7454,14 @@
       <c r="G190">
         <v>10</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I190" t="s">
+        <v>230</v>
+      </c>
+      <c r="J190" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>141</v>
       </c>
@@ -6706,8 +7483,14 @@
       <c r="G191">
         <v>10</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I191" t="s">
+        <v>294</v>
+      </c>
+      <c r="J191" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>143</v>
       </c>
@@ -6729,8 +7512,14 @@
       <c r="G192">
         <v>10</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I192" t="s">
+        <v>230</v>
+      </c>
+      <c r="J192" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>147</v>
       </c>
@@ -6752,8 +7541,14 @@
       <c r="G193">
         <v>10</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I193" t="s">
+        <v>230</v>
+      </c>
+      <c r="J193" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>169</v>
       </c>
@@ -6775,8 +7570,14 @@
       <c r="G194">
         <v>10</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I194" t="s">
+        <v>230</v>
+      </c>
+      <c r="J194" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>171</v>
       </c>
@@ -6798,8 +7599,14 @@
       <c r="G195">
         <v>10</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I195" t="s">
+        <v>230</v>
+      </c>
+      <c r="J195" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>175</v>
       </c>
@@ -6821,8 +7628,14 @@
       <c r="G196">
         <v>10</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I196" t="s">
+        <v>230</v>
+      </c>
+      <c r="J196" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>179</v>
       </c>
@@ -6844,8 +7657,14 @@
       <c r="G197">
         <v>10</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I197" t="s">
+        <v>230</v>
+      </c>
+      <c r="J197" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>185</v>
       </c>
@@ -6867,8 +7686,14 @@
       <c r="G198">
         <v>10</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I198" t="s">
+        <v>230</v>
+      </c>
+      <c r="J198" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>189</v>
       </c>
@@ -6890,8 +7715,14 @@
       <c r="G199">
         <v>10</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I199" t="s">
+        <v>230</v>
+      </c>
+      <c r="J199" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>193</v>
       </c>
@@ -6913,8 +7744,14 @@
       <c r="G200">
         <v>10</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I200" t="s">
+        <v>230</v>
+      </c>
+      <c r="J200" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>203</v>
       </c>
@@ -6936,8 +7773,14 @@
       <c r="G201">
         <v>10</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I201" t="s">
+        <v>230</v>
+      </c>
+      <c r="J201" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -6959,8 +7802,14 @@
       <c r="G202">
         <v>10</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I202" t="s">
+        <v>230</v>
+      </c>
+      <c r="J202" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>209</v>
       </c>
@@ -6982,8 +7831,14 @@
       <c r="G203">
         <v>10</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I203" t="s">
+        <v>230</v>
+      </c>
+      <c r="J203" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>213</v>
       </c>
@@ -7005,8 +7860,14 @@
       <c r="G204">
         <v>10</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I204" t="s">
+        <v>294</v>
+      </c>
+      <c r="J204" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>217</v>
       </c>
@@ -7028,8 +7889,14 @@
       <c r="G205">
         <v>10</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I205" t="s">
+        <v>230</v>
+      </c>
+      <c r="J205" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>221</v>
       </c>
@@ -7051,8 +7918,14 @@
       <c r="G206">
         <v>10</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I206" t="s">
+        <v>230</v>
+      </c>
+      <c r="J206" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>223</v>
       </c>
@@ -7074,8 +7947,14 @@
       <c r="G207">
         <v>10</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I207" t="s">
+        <v>294</v>
+      </c>
+      <c r="J207" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>225</v>
       </c>
@@ -7097,8 +7976,14 @@
       <c r="G208">
         <v>10</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I208" t="s">
+        <v>230</v>
+      </c>
+      <c r="J208" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>240</v>
       </c>
@@ -7120,8 +8005,14 @@
       <c r="G209">
         <v>10</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I209" t="s">
+        <v>230</v>
+      </c>
+      <c r="J209" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>242</v>
       </c>
@@ -7143,8 +8034,14 @@
       <c r="G210">
         <v>10</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I210" t="s">
+        <v>230</v>
+      </c>
+      <c r="J210" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>244</v>
       </c>
@@ -7166,8 +8063,14 @@
       <c r="G211">
         <v>10</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I211" t="s">
+        <v>230</v>
+      </c>
+      <c r="J211" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>246</v>
       </c>
@@ -7189,8 +8092,14 @@
       <c r="G212">
         <v>10</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I212" t="s">
+        <v>294</v>
+      </c>
+      <c r="J212" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>252</v>
       </c>
@@ -7212,8 +8121,14 @@
       <c r="G213">
         <v>10</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I213" t="s">
+        <v>230</v>
+      </c>
+      <c r="J213" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>254</v>
       </c>
@@ -7235,8 +8150,14 @@
       <c r="G214">
         <v>10</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I214" t="s">
+        <v>230</v>
+      </c>
+      <c r="J214" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>256</v>
       </c>
@@ -7258,8 +8179,14 @@
       <c r="G215">
         <v>10</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I215" t="s">
+        <v>230</v>
+      </c>
+      <c r="J215" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>270</v>
       </c>
@@ -7281,8 +8208,14 @@
       <c r="G216">
         <v>10</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I216" t="s">
+        <v>230</v>
+      </c>
+      <c r="J216" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>274</v>
       </c>
@@ -7304,8 +8237,14 @@
       <c r="G217">
         <v>10</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I217" t="s">
+        <v>230</v>
+      </c>
+      <c r="J217" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>276</v>
       </c>
@@ -7327,8 +8266,14 @@
       <c r="G218">
         <v>10</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I218" t="s">
+        <v>230</v>
+      </c>
+      <c r="J218" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>286</v>
       </c>
@@ -7350,8 +8295,14 @@
       <c r="G219">
         <v>10</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I219" t="s">
+        <v>230</v>
+      </c>
+      <c r="J219" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>288</v>
       </c>
@@ -7373,8 +8324,14 @@
       <c r="G220">
         <v>10</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I220" t="s">
+        <v>230</v>
+      </c>
+      <c r="J220" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>298</v>
       </c>
@@ -7396,8 +8353,14 @@
       <c r="G221">
         <v>10</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I221" t="s">
+        <v>230</v>
+      </c>
+      <c r="J221" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>300</v>
       </c>
@@ -7419,8 +8382,14 @@
       <c r="G222">
         <v>10</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I222" t="s">
+        <v>230</v>
+      </c>
+      <c r="J222" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>306</v>
       </c>
@@ -7442,8 +8411,14 @@
       <c r="G223">
         <v>10</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I223" t="s">
+        <v>230</v>
+      </c>
+      <c r="J223" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>308</v>
       </c>
@@ -7465,8 +8440,14 @@
       <c r="G224">
         <v>10</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I224" t="s">
+        <v>230</v>
+      </c>
+      <c r="J224" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>310</v>
       </c>
@@ -7488,8 +8469,14 @@
       <c r="G225">
         <v>10</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I225" t="s">
+        <v>230</v>
+      </c>
+      <c r="J225" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>330</v>
       </c>
@@ -7511,8 +8498,14 @@
       <c r="G226">
         <v>10</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I226" t="s">
+        <v>230</v>
+      </c>
+      <c r="J226" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>334</v>
       </c>
@@ -7534,8 +8527,14 @@
       <c r="G227">
         <v>10</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I227" t="s">
+        <v>294</v>
+      </c>
+      <c r="J227" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>336</v>
       </c>
@@ -7557,8 +8556,14 @@
       <c r="G228">
         <v>10</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I228" t="s">
+        <v>230</v>
+      </c>
+      <c r="J228" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>338</v>
       </c>
@@ -7580,8 +8585,14 @@
       <c r="G229">
         <v>10</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I229" t="s">
+        <v>230</v>
+      </c>
+      <c r="J229" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>348</v>
       </c>
@@ -7603,8 +8614,14 @@
       <c r="G230">
         <v>10</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I230" t="s">
+        <v>230</v>
+      </c>
+      <c r="J230" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>354</v>
       </c>
@@ -7626,8 +8643,14 @@
       <c r="G231">
         <v>10</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I231" t="s">
+        <v>230</v>
+      </c>
+      <c r="J231" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>360</v>
       </c>
@@ -7649,8 +8672,14 @@
       <c r="G232">
         <v>10</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I232" t="s">
+        <v>230</v>
+      </c>
+      <c r="J232" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>364</v>
       </c>
@@ -7672,8 +8701,14 @@
       <c r="G233">
         <v>10</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I233" t="s">
+        <v>230</v>
+      </c>
+      <c r="J233" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>366</v>
       </c>
@@ -7695,8 +8730,14 @@
       <c r="G234">
         <v>10</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I234" t="s">
+        <v>294</v>
+      </c>
+      <c r="J234" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>368</v>
       </c>
@@ -7718,8 +8759,14 @@
       <c r="G235">
         <v>10</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I235" t="s">
+        <v>230</v>
+      </c>
+      <c r="J235" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>370</v>
       </c>
@@ -7741,8 +8788,14 @@
       <c r="G236">
         <v>10</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I236" t="s">
+        <v>230</v>
+      </c>
+      <c r="J236" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>374</v>
       </c>
@@ -7764,8 +8817,14 @@
       <c r="G237">
         <v>10</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I237" t="s">
+        <v>230</v>
+      </c>
+      <c r="J237" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>376</v>
       </c>
@@ -7787,8 +8846,14 @@
       <c r="G238">
         <v>10</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I238" t="s">
+        <v>230</v>
+      </c>
+      <c r="J238" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>378</v>
       </c>
@@ -7810,8 +8875,14 @@
       <c r="G239">
         <v>10</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I239" t="s">
+        <v>230</v>
+      </c>
+      <c r="J239" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>380</v>
       </c>
@@ -7833,8 +8904,14 @@
       <c r="G240">
         <v>10</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I240" t="s">
+        <v>294</v>
+      </c>
+      <c r="J240" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>382</v>
       </c>
@@ -7856,8 +8933,14 @@
       <c r="G241">
         <v>10</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I241" t="s">
+        <v>230</v>
+      </c>
+      <c r="J241" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>384</v>
       </c>
@@ -7879,8 +8962,14 @@
       <c r="G242">
         <v>10</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I242" t="s">
+        <v>230</v>
+      </c>
+      <c r="J242" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>386</v>
       </c>
@@ -7902,8 +8991,14 @@
       <c r="G243">
         <v>10</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I243" t="s">
+        <v>230</v>
+      </c>
+      <c r="J243" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>388</v>
       </c>
@@ -7925,8 +9020,14 @@
       <c r="G244">
         <v>10</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I244" t="s">
+        <v>230</v>
+      </c>
+      <c r="J244" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>394</v>
       </c>
@@ -7948,8 +9049,14 @@
       <c r="G245">
         <v>10</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I245" t="s">
+        <v>230</v>
+      </c>
+      <c r="J245" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>396</v>
       </c>
@@ -7971,8 +9078,14 @@
       <c r="G246">
         <v>10</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I246" t="s">
+        <v>230</v>
+      </c>
+      <c r="J246" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>400</v>
       </c>
@@ -7994,8 +9107,14 @@
       <c r="G247">
         <v>10</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I247" t="s">
+        <v>230</v>
+      </c>
+      <c r="J247" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>402</v>
       </c>
@@ -8017,8 +9136,14 @@
       <c r="G248">
         <v>10</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I248" t="s">
+        <v>230</v>
+      </c>
+      <c r="J248" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>404</v>
       </c>
@@ -8040,8 +9165,14 @@
       <c r="G249">
         <v>10</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I249" t="s">
+        <v>230</v>
+      </c>
+      <c r="J249" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>406</v>
       </c>
@@ -8063,8 +9194,14 @@
       <c r="G250">
         <v>10</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I250" t="s">
+        <v>230</v>
+      </c>
+      <c r="J250" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>408</v>
       </c>
@@ -8086,8 +9223,14 @@
       <c r="G251">
         <v>10</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I251" t="s">
+        <v>230</v>
+      </c>
+      <c r="J251" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>412</v>
       </c>
@@ -8109,8 +9252,14 @@
       <c r="G252">
         <v>10</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I252" t="s">
+        <v>230</v>
+      </c>
+      <c r="J252" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>414</v>
       </c>
@@ -8132,8 +9281,14 @@
       <c r="G253">
         <v>10</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I253" t="s">
+        <v>230</v>
+      </c>
+      <c r="J253" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>418</v>
       </c>
@@ -8155,8 +9310,14 @@
       <c r="G254">
         <v>10</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I254" t="s">
+        <v>230</v>
+      </c>
+      <c r="J254" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>422</v>
       </c>
@@ -8178,8 +9339,14 @@
       <c r="G255">
         <v>10</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I255" t="s">
+        <v>230</v>
+      </c>
+      <c r="J255" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>424</v>
       </c>
@@ -8201,8 +9368,14 @@
       <c r="G256">
         <v>10</v>
       </c>
-    </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I256" t="s">
+        <v>230</v>
+      </c>
+      <c r="J256" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>432</v>
       </c>
@@ -8224,8 +9397,14 @@
       <c r="G257">
         <v>10</v>
       </c>
-    </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I257" t="s">
+        <v>230</v>
+      </c>
+      <c r="J257" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>438</v>
       </c>
@@ -8247,8 +9426,14 @@
       <c r="G258">
         <v>10</v>
       </c>
-    </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I258" t="s">
+        <v>230</v>
+      </c>
+      <c r="J258" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>440</v>
       </c>
@@ -8270,8 +9455,14 @@
       <c r="G259">
         <v>10</v>
       </c>
-    </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I259" t="s">
+        <v>230</v>
+      </c>
+      <c r="J259" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>442</v>
       </c>
@@ -8293,8 +9484,14 @@
       <c r="G260">
         <v>10</v>
       </c>
-    </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I260" t="s">
+        <v>230</v>
+      </c>
+      <c r="J260" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>446</v>
       </c>
@@ -8316,8 +9513,14 @@
       <c r="G261">
         <v>10</v>
       </c>
-    </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I261" t="s">
+        <v>230</v>
+      </c>
+      <c r="J261" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>448</v>
       </c>
@@ -8339,8 +9542,14 @@
       <c r="G262">
         <v>10</v>
       </c>
-    </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I262" t="s">
+        <v>230</v>
+      </c>
+      <c r="J262" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>450</v>
       </c>
@@ -8362,8 +9571,14 @@
       <c r="G263">
         <v>10</v>
       </c>
-    </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I263" t="s">
+        <v>230</v>
+      </c>
+      <c r="J263" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>454</v>
       </c>
@@ -8385,8 +9600,14 @@
       <c r="G264">
         <v>10</v>
       </c>
-    </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I264" t="s">
+        <v>230</v>
+      </c>
+      <c r="J264" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>456</v>
       </c>
@@ -8408,8 +9629,14 @@
       <c r="G265">
         <v>10</v>
       </c>
-    </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I265" t="s">
+        <v>230</v>
+      </c>
+      <c r="J265" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>460</v>
       </c>
@@ -8431,8 +9658,14 @@
       <c r="G266">
         <v>10</v>
       </c>
-    </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I266" t="s">
+        <v>230</v>
+      </c>
+      <c r="J266" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>462</v>
       </c>
@@ -8454,8 +9687,14 @@
       <c r="G267">
         <v>10</v>
       </c>
-    </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I267" t="s">
+        <v>230</v>
+      </c>
+      <c r="J267" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>468</v>
       </c>
@@ -8477,8 +9716,14 @@
       <c r="G268">
         <v>10</v>
       </c>
-    </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I268" t="s">
+        <v>230</v>
+      </c>
+      <c r="J268" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>470</v>
       </c>
@@ -8500,8 +9745,14 @@
       <c r="G269">
         <v>10</v>
       </c>
-    </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I269" t="s">
+        <v>230</v>
+      </c>
+      <c r="J269" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>472</v>
       </c>
@@ -8523,8 +9774,14 @@
       <c r="G270">
         <v>10</v>
       </c>
-    </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I270" t="s">
+        <v>230</v>
+      </c>
+      <c r="J270" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>488</v>
       </c>
@@ -8546,8 +9803,14 @@
       <c r="G271">
         <v>10</v>
       </c>
-    </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I271" t="s">
+        <v>230</v>
+      </c>
+      <c r="J271" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>500</v>
       </c>
@@ -8569,8 +9832,14 @@
       <c r="G272">
         <v>10</v>
       </c>
-    </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I272" t="s">
+        <v>230</v>
+      </c>
+      <c r="J272" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>502</v>
       </c>
@@ -8592,8 +9861,14 @@
       <c r="G273">
         <v>10</v>
       </c>
-    </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I273" t="s">
+        <v>230</v>
+      </c>
+      <c r="J273" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>504</v>
       </c>
@@ -8615,8 +9890,14 @@
       <c r="G274">
         <v>10</v>
       </c>
-    </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I274" t="s">
+        <v>230</v>
+      </c>
+      <c r="J274" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>508</v>
       </c>
@@ -8638,8 +9919,14 @@
       <c r="G275">
         <v>10</v>
       </c>
-    </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I275" t="s">
+        <v>230</v>
+      </c>
+      <c r="J275" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>514</v>
       </c>
@@ -8661,8 +9948,14 @@
       <c r="G276">
         <v>10</v>
       </c>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I276" t="s">
+        <v>230</v>
+      </c>
+      <c r="J276" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>518</v>
       </c>
@@ -8684,8 +9977,14 @@
       <c r="G277">
         <v>10</v>
       </c>
-    </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I277" t="s">
+        <v>230</v>
+      </c>
+      <c r="J277" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>520</v>
       </c>
@@ -8707,8 +10006,14 @@
       <c r="G278">
         <v>10</v>
       </c>
-    </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I278" t="s">
+        <v>294</v>
+      </c>
+      <c r="J278" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>522</v>
       </c>
@@ -8730,8 +10035,14 @@
       <c r="G279">
         <v>10</v>
       </c>
-    </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I279" t="s">
+        <v>230</v>
+      </c>
+      <c r="J279" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>524</v>
       </c>
@@ -8753,8 +10064,14 @@
       <c r="G280">
         <v>10</v>
       </c>
-    </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I280" t="s">
+        <v>230</v>
+      </c>
+      <c r="J280" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>526</v>
       </c>
@@ -8776,8 +10093,14 @@
       <c r="G281">
         <v>10</v>
       </c>
-    </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I281" t="s">
+        <v>230</v>
+      </c>
+      <c r="J281" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>539</v>
       </c>
@@ -8799,8 +10122,14 @@
       <c r="G282">
         <v>10</v>
       </c>
-    </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I282" t="s">
+        <v>230</v>
+      </c>
+      <c r="J282" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>555</v>
       </c>
@@ -8822,8 +10151,14 @@
       <c r="G283">
         <v>10</v>
       </c>
-    </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I283" t="s">
+        <v>230</v>
+      </c>
+      <c r="J283" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>561</v>
       </c>
@@ -8845,8 +10180,14 @@
       <c r="G284">
         <v>10</v>
       </c>
-    </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I284" t="s">
+        <v>230</v>
+      </c>
+      <c r="J284" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>567</v>
       </c>
@@ -8868,8 +10209,14 @@
       <c r="G285">
         <v>10</v>
       </c>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I285" t="s">
+        <v>230</v>
+      </c>
+      <c r="J285" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>569</v>
       </c>
@@ -8891,8 +10238,14 @@
       <c r="G286">
         <v>10</v>
       </c>
-    </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I286" t="s">
+        <v>294</v>
+      </c>
+      <c r="J286" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>571</v>
       </c>
@@ -8913,6 +10266,12 @@
       </c>
       <c r="G287">
         <v>10</v>
+      </c>
+      <c r="I287" t="s">
+        <v>230</v>
+      </c>
+      <c r="J287" t="s">
+        <v>585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>